<commit_message>
Added label change Ridesharing, fix for fabscrapdiversion, and accounting for biogenic CO2 in GWP of wood.
</commit_message>
<xml_diff>
--- a/RECC_ModelConfig_List_V2_1.xlsx
+++ b/RECC_ModelConfig_List_V2_1.xlsx
@@ -15,13 +15,14 @@
     <sheet name="GroupTestRun" sheetId="3" r:id="rId6"/>
     <sheet name="Evaluate_GroupTestRun" sheetId="7" r:id="rId7"/>
     <sheet name="Dump" sheetId="8" r:id="rId8"/>
+    <sheet name="Dump2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2233" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="260">
   <si>
     <t>Sheet_Name</t>
   </si>
@@ -656,15 +657,9 @@
     <t>Germany_passvehivles_SensAn</t>
   </si>
   <si>
-    <t>RECC_Germany_2019_8_8__6_41_6_PassVehs</t>
-  </si>
-  <si>
     <t>RECC_Germany_2019_8_8__6_41_43_PassVehs_FYI</t>
   </si>
   <si>
-    <t>RECC_Germany_2019_8_8__6_42_23_PassVehs_FSD</t>
-  </si>
-  <si>
     <t>RECC_Germany_2019_8_8__6_43_7_PassVehs_EoL</t>
   </si>
   <si>
@@ -698,15 +693,9 @@
     <t>['reb']</t>
   </si>
   <si>
-    <t>RECC_Germany_2019_8_8__6_51_36_ResBlds</t>
-  </si>
-  <si>
     <t>RECC_Germany_2019_8_8__6_52_14_ResBlds_FYI</t>
   </si>
   <si>
-    <t>RECC_Germany_2019_8_8__6_52_54_ResBlds_FSD</t>
-  </si>
-  <si>
     <t>RECC_Germany_2019_8_8__6_53_36_ResBlds_EoL</t>
   </si>
   <si>
@@ -726,6 +715,93 @@
   </si>
   <si>
     <t>RECC_Germany_2019_8_8__6_57_43_ResBlds_NoR</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_8__12_49_8_ResBlds_FSD</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_8__12_49_51_PassVehs_FSD</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_8__12_55_4_ResBlds</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_8__12_55_43_PassVehs</t>
+  </si>
+  <si>
+    <t>RiS</t>
+  </si>
+  <si>
+    <t>Germany_resbuildings_SensAn</t>
+  </si>
+  <si>
+    <t>Germany_passvehicles_SensAn</t>
+  </si>
+  <si>
+    <t>Include_REStrategy_RideSharing</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_13_16_ResBlds</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_13_55_ResBlds_FYI</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_14_33_ResBlds_FSD</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_15_11_ResBlds_EoL</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_15_48_ResBlds_MSU</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_16_26_ResBlds_ULD</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_17_4_ResBlds_RUS</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_17_46_ResBlds_LTE</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_18_34_ResBlds_MIU</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_19_19_ResBlds_NoR</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_20_3_PassVehs</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_20_42_PassVehs_FYI</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_21_24_PassVehs_FSD</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_22_4_PassVehs_EoL</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_22_45_PassVehs_MSU</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_23_26_PassVehs_ULD</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_24_7_PassVehs_RUS</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_24_47_PassVehs_LTE</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_25_28_PassVehs_CaS</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_26_9_PassVehs_RiS</t>
+  </si>
+  <si>
+    <t>RECC_Germany_2019_8_9__4_26_50_PassVehs_NoR</t>
   </si>
 </sst>
 </file>
@@ -6842,8 +6918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:S4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7036,10 +7112,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S13"/>
+  <dimension ref="B2:S24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:R2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7082,7 +7158,7 @@
         <v>206</v>
       </c>
       <c r="N2" t="s">
-        <v>207</v>
+        <v>235</v>
       </c>
       <c r="O2" t="s">
         <v>208</v>
@@ -7135,7 +7211,7 @@
         <v>200</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>201</v>
+        <v>238</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>202</v>
@@ -7155,13 +7231,13 @@
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -7214,7 +7290,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -7267,7 +7343,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -7320,7 +7396,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -7373,7 +7449,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -7426,7 +7502,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -7479,7 +7555,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -7532,7 +7608,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -7585,7 +7661,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -7638,7 +7714,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -7683,6 +7759,592 @@
         <v>14</v>
       </c>
       <c r="S13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>15</v>
+      </c>
+      <c r="R15" t="s">
+        <v>15</v>
+      </c>
+      <c r="S15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>15</v>
+      </c>
+      <c r="R16" t="s">
+        <v>15</v>
+      </c>
+      <c r="S16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>15</v>
+      </c>
+      <c r="R17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>15</v>
+      </c>
+      <c r="R19" t="s">
+        <v>15</v>
+      </c>
+      <c r="S19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>203</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" t="s">
+        <v>14</v>
+      </c>
+      <c r="P20" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>15</v>
+      </c>
+      <c r="R20" t="s">
+        <v>15</v>
+      </c>
+      <c r="S20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" t="s">
+        <v>14</v>
+      </c>
+      <c r="P21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R21" t="s">
+        <v>15</v>
+      </c>
+      <c r="S21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" t="s">
+        <v>15</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" t="s">
+        <v>14</v>
+      </c>
+      <c r="P22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" t="s">
+        <v>15</v>
+      </c>
+      <c r="O23" t="s">
+        <v>14</v>
+      </c>
+      <c r="P23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" t="s">
+        <v>15</v>
+      </c>
+      <c r="S23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" t="s">
+        <v>14</v>
+      </c>
+      <c r="P24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" t="s">
+        <v>14</v>
+      </c>
+      <c r="S24" t="s">
         <v>197</v>
       </c>
     </row>
@@ -7696,7 +8358,7 @@
   <dimension ref="B1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7720,116 +8382,116 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
-        <v>213</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>221</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>223</v>
-      </c>
       <c r="D13" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.45">
@@ -7844,701 +8506,1386 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R14"/>
+  <dimension ref="A2:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>206</v>
+      </c>
+      <c r="M2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N2" t="s">
+        <v>208</v>
+      </c>
+      <c r="O2" t="s">
+        <v>205</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>15</v>
+      </c>
+      <c r="R15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>15</v>
+      </c>
+      <c r="R16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P17" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>15</v>
+      </c>
+      <c r="R17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" t="s">
+        <v>15</v>
+      </c>
+      <c r="P19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>15</v>
+      </c>
+      <c r="R19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" t="s">
+        <v>15</v>
+      </c>
+      <c r="P20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>15</v>
+      </c>
+      <c r="R20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>203</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" t="s">
+        <v>15</v>
+      </c>
+      <c r="P22" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>203</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" t="s">
+        <v>14</v>
+      </c>
+      <c r="O23" t="s">
+        <v>15</v>
+      </c>
+      <c r="P23" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" t="s">
+        <v>14</v>
+      </c>
+      <c r="P24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>206</v>
-      </c>
-      <c r="M2" t="s">
-        <v>207</v>
-      </c>
-      <c r="N2" t="s">
-        <v>208</v>
-      </c>
-      <c r="O2" t="s">
-        <v>205</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>203</v>
-      </c>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>203</v>
-      </c>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>15</v>
-      </c>
-      <c r="R5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>203</v>
-      </c>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N6" t="s">
-        <v>14</v>
-      </c>
-      <c r="O6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>203</v>
-      </c>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" t="s">
-        <v>15</v>
-      </c>
-      <c r="P7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>203</v>
-      </c>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>15</v>
-      </c>
-      <c r="R8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>203</v>
-      </c>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" t="s">
-        <v>15</v>
-      </c>
-      <c r="P9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>203</v>
-      </c>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" t="s">
-        <v>14</v>
-      </c>
-      <c r="N10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>15</v>
-      </c>
-      <c r="R10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>203</v>
-      </c>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" t="s">
-        <v>15</v>
-      </c>
-      <c r="P11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>15</v>
-      </c>
-      <c r="R11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>203</v>
-      </c>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>15</v>
-      </c>
-      <c r="R12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" t="s">
-        <v>15</v>
-      </c>
-      <c r="P13" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>15</v>
-      </c>
-      <c r="R13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>203</v>
-      </c>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" t="s">
-        <v>14</v>
-      </c>
-      <c r="P14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>14</v>
-      </c>
-      <c r="R14" t="s">
-        <v>197</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>